<commit_message>
11/30 lab to home
</commit_message>
<xml_diff>
--- a/piModle.xlsx
+++ b/piModle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\my_First_Excelize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\PI_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF2ED7B-3419-4385-81EB-CB76A77D8E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64099171-360F-4236-A054-C603E2DB121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>SIZE</t>
-  </si>
-  <si>
-    <t>QUANTITY</t>
   </si>
   <si>
     <t>UNIT PRICE</t>
@@ -262,6 +259,10 @@
     <t>Seller:</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
+  <si>
+    <t>QUANTITY</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -282,14 +283,17 @@
       <sz val="28"/>
       <color rgb="FF7F7F7F"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -297,6 +301,7 @@
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -507,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -531,9 +536,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -608,19 +610,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -638,34 +658,40 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -698,23 +724,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1075,10 +1086,10 @@
     <outlinePr summaryBelow="0" summaryRight="0" showOutlineSymbols="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O993"/>
+  <dimension ref="A1:O994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1100,56 +1111,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="81.75" customHeight="1">
-      <c r="A1" s="58" t="str">
+      <c r="A1" s="65" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1171,23 +1182,23 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="27">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="1:15" ht="4.5" customHeight="1">
       <c r="A6" s="1"/>
@@ -1201,159 +1212,159 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" spans="1:15" ht="16.5">
-      <c r="A7" s="64" t="s">
-        <v>73</v>
+      <c r="A7" s="35" t="s">
+        <v>72</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="25" t="s">
-        <v>70</v>
+      <c r="C7" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="63" t="s">
-        <v>69</v>
+      <c r="H7" s="58"/>
+      <c r="I7" s="70" t="s">
+        <v>68</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="1:15" ht="16.5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="5"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="9" spans="1:15" ht="16.5">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="54" t="s">
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="47"/>
-      <c r="I9" s="56" t="s">
-        <v>46</v>
+      <c r="H9" s="58"/>
+      <c r="I9" s="63" t="s">
+        <v>45</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
     </row>
     <row r="10" spans="1:15" ht="16.5">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>42</v>
+      <c r="C10" s="50" t="s">
+        <v>41</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="1:15" ht="16.5">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>43</v>
+      <c r="C11" s="50" t="s">
+        <v>42</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
     </row>
     <row r="12" spans="1:15" ht="16.5">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>44</v>
+      <c r="C12" s="28" t="s">
+        <v>43</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="7"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:15" ht="9.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23" t="s">
-        <v>45</v>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22" t="s">
+        <v>44</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1365,13 +1376,13 @@
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1398,215 +1409,215 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="12.75" customHeight="1">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="9" t="s">
+      <c r="E17" s="54"/>
+      <c r="F17" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="46"/>
+      <c r="K17" s="54"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" ht="12.75" customHeight="1">
-      <c r="A18" s="52"/>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="56"/>
+      <c r="B18" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53" t="s">
+      <c r="E18" s="56"/>
+      <c r="F18" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="28" t="s">
+      <c r="G18" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="56"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="16.5">
-      <c r="A19" s="33">
+      <c r="A19" s="32">
         <v>1</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="32">
+        <v>12</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="39">
+        <v>2175</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" s="39">
+        <v>26100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16.5">
+      <c r="A20" s="32">
+        <v>3</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33">
-        <v>12</v>
+      <c r="C20" s="32" t="s">
+        <v>47</v>
       </c>
-      <c r="G19" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="69">
-        <v>2175</v>
-      </c>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="K19" s="69">
-        <v>26100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="16.5">
-      <c r="A20" s="33">
-        <v>3</v>
-      </c>
-      <c r="B20" s="33" t="s">
+      <c r="D20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="33" t="s">
-        <v>48</v>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32">
+        <v>5</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="G20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="32">
+        <v>2390</v>
+      </c>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="32">
+        <v>11950</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="16.5">
+      <c r="A21" s="32">
+        <v>4</v>
+      </c>
+      <c r="B21" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33">
-        <v>5</v>
+      <c r="C21" s="32" t="s">
+        <v>47</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>72</v>
+      <c r="D21" s="32" t="s">
+        <v>52</v>
       </c>
-      <c r="H20" s="33">
-        <v>2390</v>
-      </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="K20" s="33">
-        <v>11950</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="16.5">
-      <c r="A21" s="33">
+      <c r="E21" s="32"/>
+      <c r="F21" s="32">
         <v>4</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>52</v>
+      <c r="G21" s="32" t="s">
+        <v>71</v>
       </c>
-      <c r="C21" s="33" t="s">
-        <v>48</v>
+      <c r="H21" s="32">
+        <v>2300</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>53</v>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32" t="s">
+        <v>71</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33">
+      <c r="K21" s="32">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="16.5">
+      <c r="A22" s="32">
+        <v>2</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32">
         <v>4</v>
       </c>
-      <c r="G21" s="33" t="s">
-        <v>72</v>
+      <c r="G22" s="32" t="s">
+        <v>71</v>
       </c>
-      <c r="H21" s="33">
-        <v>2300</v>
-      </c>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="K21" s="33">
-        <v>9200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="16.5">
-      <c r="A22" s="33">
-        <v>2</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33">
-        <v>4</v>
-      </c>
-      <c r="G22" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="33">
+      <c r="H22" s="32">
         <v>2190</v>
       </c>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33" t="s">
-        <v>72</v>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32" t="s">
+        <v>71</v>
       </c>
-      <c r="K22" s="33">
+      <c r="K22" s="32">
         <v>8760</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="16.5">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" ht="18" customHeight="1">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66" t="s">
-        <v>23</v>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37" t="s">
+        <v>22</v>
       </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="31"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1620,17 +1631,17 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="10"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="9"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" ht="9" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1645,19 +1656,19 @@
     </row>
     <row r="27" spans="1:14" ht="13.5" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="50" t="s">
-        <v>54</v>
+      <c r="C27" s="49" t="s">
+        <v>53</v>
       </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1665,19 +1676,19 @@
     </row>
     <row r="28" spans="1:14" ht="13.5" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="50" t="s">
-        <v>55</v>
+      <c r="C28" s="49" t="s">
+        <v>54</v>
       </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1685,11 +1696,11 @@
     </row>
     <row r="29" spans="1:14" ht="13.5" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1704,11 +1715,11 @@
     </row>
     <row r="30" spans="1:14" ht="13.5" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1723,11 +1734,11 @@
     </row>
     <row r="31" spans="1:14" ht="13.5" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1742,18 +1753,18 @@
     </row>
     <row r="32" spans="1:14" ht="13.5" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="36" t="s">
-        <v>59</v>
+      <c r="C32" s="50" t="s">
+        <v>58</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1761,11 +1772,11 @@
     </row>
     <row r="33" spans="1:14" ht="13.5" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1780,11 +1791,11 @@
     </row>
     <row r="34" spans="1:14" ht="13.5" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1799,14 +1810,14 @@
     </row>
     <row r="35" spans="1:14" ht="13.5" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1818,14 +1829,14 @@
     </row>
     <row r="36" spans="1:14" ht="13.5" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1836,59 +1847,59 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A37" s="36" t="s">
-        <v>34</v>
+      <c r="A37" s="50" t="s">
+        <v>33</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" spans="1:14" s="22" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A38" s="36"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
+    <row r="38" spans="1:14" s="21" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A38" s="50"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="1:14" ht="7.5" customHeight="1" thickBot="1">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1902,162 +1913,162 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A41" s="14" t="s">
-        <v>35</v>
+      <c r="A41" s="13" t="s">
+        <v>34</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="37" t="s">
-        <v>64</v>
+      <c r="B41" s="14"/>
+      <c r="C41" s="51" t="s">
+        <v>63</v>
       </c>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="15"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="14"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A42" s="16" t="s">
-        <v>36</v>
+      <c r="A42" s="15" t="s">
+        <v>35</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="39" t="s">
-        <v>65</v>
+      <c r="B42" s="16"/>
+      <c r="C42" s="44" t="s">
+        <v>64</v>
       </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="17"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="16"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A43" s="16" t="s">
-        <v>37</v>
+      <c r="A43" s="15" t="s">
+        <v>36</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="39" t="s">
-        <v>66</v>
+      <c r="B43" s="16"/>
+      <c r="C43" s="44" t="s">
+        <v>65</v>
       </c>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="17"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="16"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A44" s="16" t="s">
-        <v>38</v>
+      <c r="A44" s="15" t="s">
+        <v>37</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="39" t="s">
-        <v>67</v>
+      <c r="B44" s="16"/>
+      <c r="C44" s="44" t="s">
+        <v>66</v>
       </c>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="17"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="16"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:14" ht="17.25" thickBot="1">
-      <c r="A45" s="18" t="s">
-        <v>39</v>
+      <c r="A45" s="17" t="s">
+        <v>38</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="41" t="s">
-        <v>68</v>
+      <c r="B45" s="18"/>
+      <c r="C45" s="46" t="s">
+        <v>67</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="19"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="18"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="N45" s="25"/>
-    </row>
-    <row r="46" spans="1:14" s="22" customFormat="1" ht="4.5" customHeight="1">
-      <c r="A46" s="32"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
+      <c r="N45" s="24"/>
+    </row>
+    <row r="46" spans="1:14" s="21" customFormat="1" ht="4.5" customHeight="1">
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
     </row>
     <row r="47" spans="1:14" ht="12.75" customHeight="1">
-      <c r="A47" s="20" t="s">
-        <v>40</v>
+      <c r="A47" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="24"/>
-    </row>
-    <row r="48" spans="1:14" s="22" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A48" s="43" t="s">
-        <v>71</v>
+      <c r="N47" s="23"/>
+    </row>
+    <row r="48" spans="1:14" s="21" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A48" s="48" t="s">
+        <v>70</v>
       </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
     </row>
     <row r="49" spans="1:14" ht="12.75" customHeight="1">
-      <c r="A49" s="44"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="44"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="24"/>
+      <c r="N49" s="23"/>
     </row>
     <row r="50" spans="1:14" ht="12.75" customHeight="1">
       <c r="B50" s="2"/>
@@ -2075,8 +2086,8 @@
       <c r="N50" s="1"/>
     </row>
     <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="21" t="s">
-        <v>41</v>
+      <c r="A51" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2092,55 +2103,55 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:14" ht="67.5" customHeight="1">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" ht="24.75" customHeight="1">
-      <c r="B53" s="45" t="str">
+    <row r="52" spans="1:14" s="33" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="20"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="34"/>
+      <c r="N52" s="34"/>
+    </row>
+    <row r="53" spans="1:14" ht="67.5" customHeight="1">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="1:14" ht="24.75" customHeight="1">
+      <c r="B54" s="57" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="45">
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="57">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="54"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -17169,8 +17180,24 @@
       <c r="M993" s="1"/>
       <c r="N993" s="1"/>
     </row>
+    <row r="994" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+      <c r="D994" s="1"/>
+      <c r="E994" s="1"/>
+      <c r="F994" s="1"/>
+      <c r="G994" s="1"/>
+      <c r="H994" s="1"/>
+      <c r="I994" s="1"/>
+      <c r="J994" s="1"/>
+      <c r="K994" s="1"/>
+      <c r="L994" s="1"/>
+      <c r="M994" s="1"/>
+      <c r="N994" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -17182,28 +17209,22 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="L13:N13"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="G53:K53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="G54:K54"/>
     <mergeCell ref="A37:B39"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="C27:J27"/>
     <mergeCell ref="C28:J28"/>
     <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C39:J39"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C45:J45"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C38:H38"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -17211,6 +17232,13 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C45:J45"/>
+    <mergeCell ref="A48:K48"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>

</xml_diff>